<commit_message>
Minor changes to crosswalks
</commit_message>
<xml_diff>
--- a/crosswalks/Estuarine-IUCNGET/Estuarine-IUCNGET.xlsx
+++ b/crosswalks/Estuarine-IUCNGET/Estuarine-IUCNGET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Documents\NEAP\Ecosystem-Typology\crosswalks\Estuarine-IUCNGET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A21DD9-F3A7-43C3-B746-00ED9338D7E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AC6B56-80F6-4B26-972A-FDEEECE8E3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>subject_id</t>
   </si>
@@ -117,9 +117,6 @@
     <t>estuarine: TBA</t>
   </si>
   <si>
-    <t>skos:closematch</t>
-  </si>
-  <si>
     <t>FM1.2 Permanently open riverine estuaries and bays</t>
   </si>
   <si>
@@ -133,6 +130,15 @@
   </si>
   <si>
     <t>mapping_set_id: http://w3id.org/env/crosswalk/nesp2get/2024-05-10</t>
+  </si>
+  <si>
+    <t>skos:narrowmatch</t>
+  </si>
+  <si>
+    <t>get:groups/M1.3</t>
+  </si>
+  <si>
+    <t>FM1.3 Intermittently closed and open lakes and lagoons</t>
   </si>
 </sst>
 </file>
@@ -209,10 +215,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -514,7 +516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DD23B2-5C24-4E92-A3A3-39F13C78738A}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -570,7 +572,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -582,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACFEC63-F603-4D93-B073-540A32B07BA6}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,19 +650,19 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -675,12 +677,40 @@
         <v>45422</v>
       </c>
       <c r="K2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G3" s="3"/>
-      <c r="I3" s="2"/>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2">
+        <v>45422</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G4" s="3"/>
@@ -800,6 +830,56 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -808,7 +888,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
@@ -825,7 +905,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -1101,57 +1181,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1159,7 +1197,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1170,7 +1208,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1187,12 +1225,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add row with correct predicates
</commit_message>
<xml_diff>
--- a/crosswalks/Estuarine-IUCNGET/Estuarine-IUCNGET.xlsx
+++ b/crosswalks/Estuarine-IUCNGET/Estuarine-IUCNGET.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Documents\NEAP\Ecosystem-Typology\crosswalks\Estuarine-IUCNGET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ecosystem-typology\crosswalks\Estuarine-IUCNGET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AC6B56-80F6-4B26-972A-FDEEECE8E3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E090BE04-7BB0-4834-8E20-FAEE8B50A419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="2340" yWindow="-16095" windowWidth="20745" windowHeight="11265" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>subject_id</t>
   </si>
@@ -114,9 +114,6 @@
     <t>author_label</t>
   </si>
   <si>
-    <t>estuarine: TBA</t>
-  </si>
-  <si>
     <t>FM1.2 Permanently open riverine estuaries and bays</t>
   </si>
   <si>
@@ -139,13 +136,61 @@
   </si>
   <si>
     <t>FM1.3 Intermittently closed and open lakes and lagoons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   estuarine: https://w3id.org/env/neap/estuarine/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   sssom: https://w3id.org/sssom/</t>
+  </si>
+  <si>
+    <t>rdf:subject</t>
+  </si>
+  <si>
+    <t>sssom:subject_label</t>
+  </si>
+  <si>
+    <t>rdf:predicate</t>
+  </si>
+  <si>
+    <t>rdf:object</t>
+  </si>
+  <si>
+    <t>sssom:object_label</t>
+  </si>
+  <si>
+    <t>sssom:mapping_justification</t>
+  </si>
+  <si>
+    <t>dcterms:creator</t>
+  </si>
+  <si>
+    <t>sssom:creator_label</t>
+  </si>
+  <si>
+    <t>dcterms:created</t>
+  </si>
+  <si>
+    <t>sssom:confidence</t>
+  </si>
+  <si>
+    <t>crosswalk:status</t>
+  </si>
+  <si>
+    <t>rdfs:comment</t>
+  </si>
+  <si>
+    <t>sssom:reviewer_id</t>
+  </si>
+  <si>
+    <t>rdfs:label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +210,32 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -190,19 +261,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{30535D9B-A7A0-4D0D-9C27-901A8F66BC18}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -514,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DD23B2-5C24-4E92-A3A3-39F13C78738A}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +616,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -560,19 +639,24 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
+    <row r="8" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -582,22 +666,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACFEC63-F603-4D93-B073-540A32B07BA6}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34" customWidth="1"/>
+    <col min="5" max="5" width="41.85546875" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
@@ -606,95 +690,107 @@
     <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="2">
-        <v>45422</v>
-      </c>
-      <c r="K2" t="s">
-        <v>27</v>
-      </c>
+      <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -709,12 +805,48 @@
         <v>45422</v>
       </c>
       <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="3" t="str">
+        <f>_xlfn.CONCAT(A3, " - mapping to IUCN GET")</f>
+        <v>estuarine:Estuarine, delta - mapping to IUCN GET</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G4" s="3"/>
-      <c r="I4" s="2"/>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2">
+        <v>45422</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="3" t="str">
+        <f>_xlfn.CONCAT(A4, " - mapping to IUCN GET")</f>
+        <v>estuarine:Estuarine, delta - mapping to IUCN GET</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G5" s="3"/>
@@ -822,6 +954,10 @@
     </row>
     <row r="31" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G31" s="3"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G32" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -830,65 +966,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
@@ -905,7 +982,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -1181,23 +1258,66 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1208,7 +1328,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1225,4 +1345,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update header sheets to work with Glenn's Python code for conversion to RDF (TTL)
</commit_message>
<xml_diff>
--- a/crosswalks/Estuarine-IUCNGET/Estuarine-IUCNGET.xlsx
+++ b/crosswalks/Estuarine-IUCNGET/Estuarine-IUCNGET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ecosystem-typology\crosswalks\Estuarine-IUCNGET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E090BE04-7BB0-4834-8E20-FAEE8B50A419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FCFCCE-C360-4079-97AF-E72622CE3BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="-16095" windowWidth="20745" windowHeight="11265" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="12570" yWindow="2595" windowWidth="19425" windowHeight="15345" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="5" r:id="rId1"/>
@@ -37,83 +37,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
-  <si>
-    <t>subject_id</t>
-  </si>
-  <si>
-    <t>subject_label</t>
-  </si>
-  <si>
-    <t>predicate_id</t>
-  </si>
-  <si>
-    <t>object_id</t>
-  </si>
-  <si>
-    <t>object_label</t>
-  </si>
-  <si>
-    <t>mapping_justification</t>
-  </si>
-  <si>
-    <t>author_id</t>
-  </si>
-  <si>
-    <t>mapping_date</t>
-  </si>
-  <si>
-    <t>confidence</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>semapv:ManualMappingCuration</t>
   </si>
   <si>
-    <t>reviewer_id</t>
-  </si>
-  <si>
     <t>orcid:0009-0001-6090-9959</t>
   </si>
   <si>
     <t>Craig Macfarlane</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>get:groups/M1.2</t>
   </si>
   <si>
-    <t>creator_id: https://orcid.org/0000-0002-3884-3420</t>
-  </si>
-  <si>
-    <t>curie_map:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   get: https://global-ecosystems.org/explore/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   skos: http://www.w3.org/2004/02/skos/core#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   semapv: https://w3id.org/semapv/vocab/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   orcid: https://orcid.org/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   status: https://w3id.org/sssom/status/</t>
-  </si>
-  <si>
-    <t>license: https://creativecommons.org/publicdomain/zero/1.0/</t>
-  </si>
-  <si>
-    <t>author_label</t>
-  </si>
-  <si>
     <t>FM1.2 Permanently open riverine estuaries and bays</t>
   </si>
   <si>
@@ -126,9 +63,6 @@
     <t>estuarine:Estuarine, delta</t>
   </si>
   <si>
-    <t>mapping_set_id: http://w3id.org/env/crosswalk/nesp2get/2024-05-10</t>
-  </si>
-  <si>
     <t>skos:narrowmatch</t>
   </si>
   <si>
@@ -138,12 +72,6 @@
     <t>FM1.3 Intermittently closed and open lakes and lagoons</t>
   </si>
   <si>
-    <t xml:space="preserve">   estuarine: https://w3id.org/env/neap/estuarine/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   sssom: https://w3id.org/sssom/</t>
-  </si>
-  <si>
     <t>rdf:subject</t>
   </si>
   <si>
@@ -184,26 +112,43 @@
   </si>
   <si>
     <t>rdfs:label</t>
+  </si>
+  <si>
+    <t>orcid: https://orcid.org/</t>
+  </si>
+  <si>
+    <t>sssom: https://w3id.org/sssom/</t>
+  </si>
+  <si>
+    <t>semapv: https://w3id.org/semapv/vocab/</t>
+  </si>
+  <si>
+    <t>crosswalk: https://w3id.org/env/neap/crosswalk/</t>
+  </si>
+  <si>
+    <t>status: https://w3id.org/env/neap/status/</t>
+  </si>
+  <si>
+    <t>get: https://global-ecosystems.org/explore/</t>
+  </si>
+  <si>
+    <t>estuarine: https://w3id.org/env/neap/estuarine/</t>
+  </si>
+  <si>
+    <t>map: http://w3id.org/env/neap/estuarine-get/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF1F2328"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -238,18 +183,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -263,21 +202,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DD23B2-5C24-4E92-A3A3-39F13C78738A}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,58 +541,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>16</v>
+      <c r="A1" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
+      <c r="A2" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>33</v>
+      <c r="A3" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
+      <c r="A4" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
+      <c r="A5" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>20</v>
+      <c r="A6" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -666,10 +587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACFEC63-F603-4D93-B073-540A32B07BA6}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,274 +611,232 @@
     <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>48</v>
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="H2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="I2" s="1">
+        <v>45422</v>
+      </c>
+      <c r="K2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="1"/>
+      <c r="N2" s="2" t="str">
+        <f>_xlfn.CONCAT(A2, " - mapping to IUCN GET")</f>
+        <v>estuarine:Estuarine, delta - mapping to IUCN GET</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="2">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1">
         <v>45422</v>
       </c>
       <c r="K3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="3" t="str">
+        <v>5</v>
+      </c>
+      <c r="N3" s="2" t="str">
         <f>_xlfn.CONCAT(A3, " - mapping to IUCN GET")</f>
         <v>estuarine:Estuarine, delta - mapping to IUCN GET</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="2">
-        <v>45422</v>
-      </c>
-      <c r="K4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="3" t="str">
-        <f>_xlfn.CONCAT(A4, " - mapping to IUCN GET")</f>
-        <v>estuarine:Estuarine, delta - mapping to IUCN GET</v>
-      </c>
+      <c r="G4" s="2"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G5" s="3"/>
-      <c r="I5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G6" s="3"/>
-      <c r="I6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G7" s="3"/>
-      <c r="I7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G8" s="3"/>
-      <c r="I8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G9" s="3"/>
-      <c r="I9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G10" s="3"/>
-      <c r="I10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G11" s="3"/>
-      <c r="I11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G12" s="3"/>
-      <c r="I12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G13" s="3"/>
-      <c r="I13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G14" s="3"/>
-      <c r="I14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G15" s="3"/>
-      <c r="I15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G16" s="3"/>
-      <c r="I16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G17" s="3"/>
-      <c r="I17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G18" s="3"/>
-      <c r="I18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="I18" s="1"/>
     </row>
     <row r="19" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G19" s="3"/>
-      <c r="I19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="I19" s="1"/>
     </row>
     <row r="20" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G20" s="3"/>
-      <c r="I20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="I20" s="1"/>
     </row>
     <row r="21" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G21" s="3"/>
-      <c r="I21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="I21" s="1"/>
     </row>
     <row r="22" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G22" s="3"/>
-      <c r="I22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="I22" s="1"/>
     </row>
     <row r="23" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G23" s="3"/>
-      <c r="I23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="I23" s="1"/>
     </row>
     <row r="24" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G24" s="3"/>
-      <c r="I24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="I24" s="1"/>
     </row>
     <row r="25" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G25" s="3"/>
-      <c r="I25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="I25" s="1"/>
     </row>
     <row r="26" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G26" s="3"/>
-      <c r="I26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="I26" s="1"/>
     </row>
     <row r="27" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G27" s="3"/>
-      <c r="I27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="I27" s="1"/>
     </row>
     <row r="28" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G28" s="3"/>
-      <c r="I28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="I28" s="1"/>
     </row>
     <row r="29" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G29" s="3"/>
-      <c r="I29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="I29" s="1"/>
     </row>
     <row r="30" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G30" s="3"/>
-      <c r="I30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="I30" s="1"/>
     </row>
     <row r="31" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G31" s="3"/>
-      <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G32" s="3"/>
+      <c r="G31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -966,23 +845,65 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
-    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
-    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
-      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
-      <Description>63P7TJYCZHM3-28990658-16955</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -1258,77 +1179,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
+    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
+    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
+      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
+      <Description>63P7TJYCZHM3-28990658-16955</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
-    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1347,18 +1231,13 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
+    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
change to esturine crosswalk line order
</commit_message>
<xml_diff>
--- a/crosswalks/Estuarine-IUCNGET/Estuarine-IUCNGET.xlsx
+++ b/crosswalks/Estuarine-IUCNGET/Estuarine-IUCNGET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/new298_csiro_au/Documents/Code/Python/NEAP/ecosystem-typology/crosswalks/Estuarine-IUCNGET/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{E6FCFCCE-C360-4079-97AF-E72622CE3BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C138EB2C-062E-4BF4-A5C1-3B2615FC4191}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{E6FCFCCE-C360-4079-97AF-E72622CE3BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D82C8FEB-4C17-4353-851A-8139A4E65A5B}"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="1512" windowWidth="33876" windowHeight="15768" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="10944" yWindow="1920" windowWidth="21792" windowHeight="14832" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="5" r:id="rId1"/>
@@ -587,10 +587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACFEC63-F603-4D93-B073-540A32B07BA6}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,10 +666,10 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -702,10 +702,10 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -833,10 +833,6 @@
     </row>
     <row r="30" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G30" s="2"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -845,6 +841,82 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
+    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
+    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
+      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
+      <Description>63P7TJYCZHM3-28990658-16955</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -1120,83 +1192,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
+    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
-    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
-    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
-      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
-      <Description>63P7TJYCZHM3-28990658-16955</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1213,31 +1236,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
-    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>